<commit_message>
Various changes and updates over the last year
Last update was Jul 18, 2022. Comiting and pushing various updates to Prioritization code.
</commit_message>
<xml_diff>
--- a/Data/Habitat_Data/Confinement_Scores.xlsx
+++ b/Data/Habitat_Data/Confinement_Scores.xlsx
@@ -24166,7 +24166,9 @@
       <c r="B724" t="s">
         <v>857</v>
       </c>
-      <c r="C724"/>
+      <c r="C724" t="s">
+        <v>16</v>
+      </c>
       <c r="D724" t="n">
         <v>0.055781</v>
       </c>
@@ -24544,9 +24546,7 @@
       <c r="B737" t="s">
         <v>867</v>
       </c>
-      <c r="C737" t="s">
-        <v>20</v>
-      </c>
+      <c r="C737"/>
       <c r="D737" t="n">
         <v>0.054725</v>
       </c>

</xml_diff>